<commit_message>
update oops and metrics
</commit_message>
<xml_diff>
--- a/metrics_labels.xlsx
+++ b/metrics_labels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eno\Documents\Git_repo\ebrahimnorouzi_github\mseo.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A288238-9548-4CC5-821D-19C5A1EF0AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102CC089-A8D7-4BF7-9F95-6C929D240582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="17460" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="93">
   <si>
     <t>selected</t>
   </si>
@@ -167,18 +167,6 @@
   </si>
   <si>
     <t xml:space="preserve">low (near 0) =&gt; poor axiomatisation&amp;#10;Higher =&gt; better&amp;#10;Extremely high = over axiomatisation </t>
-  </si>
-  <si>
-    <t>Classrelationratio</t>
-  </si>
-  <si>
-    <t>Class Relation Ratio</t>
-  </si>
-  <si>
-    <t>This metric describes the ratio between the classes and the relations in the ontology. &amp;#10;Note: The following ontology components are counted as relationships: Object Properties, Equivalent Classes, Disjoint Classes, Subclasses(Subclass of).&amp;#10;Typically good values are in the range [0.3, 0.8] indicating a sufficient number of properties connecting things with other things (i.e. object properties) and values (datatype properties).  The interpretation of the ratio always depends of the ontology size.</t>
-  </si>
-  <si>
-    <t>Low values (i.e near 0) indicate an ontology with many properties connecting few concepts. On the contrary, high values indicate an ontology with many concepts connected by few properties.</t>
   </si>
   <si>
     <t>Graphmetrics</t>
@@ -328,9 +316,6 @@
   </si>
   <si>
     <t>The value of the absolute breadth</t>
-  </si>
-  <si>
-    <t>Class/property ratio</t>
   </si>
 </sst>
 </file>
@@ -734,11 +719,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -943,16 +928,16 @@
         <v>36</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -1033,128 +1018,128 @@
         <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A15" s="2"/>
+      <c r="B15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A16" s="2"/>
-      <c r="B16" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="G17" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
@@ -1162,22 +1147,19 @@
         <v>7</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>73</v>
+        <v>49</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
@@ -1185,19 +1167,22 @@
         <v>7</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>96</v>
+        <v>49</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
@@ -1205,7 +1190,7 @@
         <v>7</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>74</v>
@@ -1214,13 +1199,13 @@
         <v>75</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
@@ -1228,46 +1213,29 @@
         <v>7</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="G22" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>84</v>
-      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A23" s="2"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A24" s="2"/>
@@ -1301,12 +1269,12 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A29" s="2"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A30" s="2"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A31" s="2"/>
@@ -1314,12 +1282,6 @@
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A32" s="2"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update the index file
</commit_message>
<xml_diff>
--- a/metrics_labels.xlsx
+++ b/metrics_labels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eno\Documents\Git_repo\ebrahimnorouzi_github\mseo.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102CC089-A8D7-4BF7-9F95-6C929D240582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C850B94-9928-441B-BBB3-D1DDA983E7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="17460" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="108">
   <si>
     <t>selected</t>
   </si>
@@ -167,6 +167,21 @@
   </si>
   <si>
     <t xml:space="preserve">low (near 0) =&gt; poor axiomatisation&amp;#10;Higher =&gt; better&amp;#10;Extremely high = over axiomatisation </t>
+  </si>
+  <si>
+    <t>Classrelationratio</t>
+  </si>
+  <si>
+    <t>Class/propery ratio</t>
+  </si>
+  <si>
+    <t>Class Relation Ratio</t>
+  </si>
+  <si>
+    <t>This metric describes the ratio between the classes and the relations in the ontology. &amp;#10;Note: The following ontology components are counted as relationships: Object Properties, Equivalent Classes, Disjoint Classes, Subclasses(Subclass of).&amp;#10;Typically good values are in the range [0.3, 0.8] indicating a sufficient number of properties connecting things with other things (i.e. object properties) and values (datatype properties).  The interpretation of the ratio always depends of the ontology size.</t>
+  </si>
+  <si>
+    <t>Low values (i.e near 0) indicate an ontology with many properties connecting few concepts. On the contrary, high values indicate an ontology with many concepts connected by few properties.</t>
   </si>
   <si>
     <t>Graphmetrics</t>
@@ -316,6 +331,36 @@
   </si>
   <si>
     <t>The value of the absolute breadth</t>
+  </si>
+  <si>
+    <t>ClassMetrics</t>
+  </si>
+  <si>
+    <t>Classconnectivity</t>
+  </si>
+  <si>
+    <t>Classfulness</t>
+  </si>
+  <si>
+    <t>Classimportance</t>
+  </si>
+  <si>
+    <t>Classinheritancerichness</t>
+  </si>
+  <si>
+    <t>Classreadability</t>
+  </si>
+  <si>
+    <t>Classrelationshiprichness</t>
+  </si>
+  <si>
+    <t>Classchildrencount</t>
+  </si>
+  <si>
+    <t>Classinstancescount</t>
+  </si>
+  <si>
+    <t>Classpropertiescount</t>
   </si>
 </sst>
 </file>
@@ -719,11 +764,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -928,16 +973,16 @@
         <v>36</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="G9" s="4"/>
     </row>
@@ -1018,46 +1063,48 @@
         <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G14" s="4" t="s">
+    </row>
+    <row r="15" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A15" s="2"/>
-      <c r="B15" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>55</v>
@@ -1076,55 +1123,53 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A16" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A16" s="2"/>
       <c r="B16" s="4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.75">
+        <v>63</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
+        <v>94</v>
+      </c>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>65</v>
@@ -1147,19 +1192,22 @@
         <v>7</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>92</v>
+        <v>54</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
@@ -1167,22 +1215,19 @@
         <v>7</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>73</v>
+        <v>54</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
@@ -1190,13 +1235,13 @@
         <v>7</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>76</v>
@@ -1205,7 +1250,7 @@
         <v>77</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
@@ -1213,74 +1258,199 @@
         <v>7</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A23" s="2"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+    </row>
+    <row r="23" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A24" s="2"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="A24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A25" s="2"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="A25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A26" s="2"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="A26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A27" s="2"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="A27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A28" s="2"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="A28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A29" s="2"/>
+      <c r="A29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A30" s="2"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+      <c r="A30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.75">
-      <c r="A31" s="2"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="A31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.75">
+      <c r="A32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>107</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>